<commit_message>
Dokument u. App bearbeitet
</commit_message>
<xml_diff>
--- a/Zeiterfassung/Zeiterfassung_Bashar_Metin.xlsx
+++ b/Zeiterfassung/Zeiterfassung_Bashar_Metin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\5.Klasse\SWP\Coding\Diplomarbeit-FahrgemeinschaftenApp\Zeiterfassung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zodia\OneDrive - HTL Dornbirn\5cWI\Z_Diplomarbeit\Diplomarbeit-FahrgemeinschaftenApp\Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE53C405-05E5-468A-A994-D96855B7C903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D4A3A-43AF-4976-9CF6-B67277B0CD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMME" sheetId="7" r:id="rId1"/>
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00762D3-10B6-4EB2-9095-A21CAC2867B8}">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -566,7 +566,7 @@
       </c>
       <c r="B3">
         <f>September!I40+Oktober!I48+November!I40+Dezember!I40+Jänner!I40+Februar!I40+März!I40</f>
-        <v>154.5</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -575,7 +575,7 @@
       </c>
       <c r="B4">
         <f>September!I41+Oktober!I49+November!I41+Dezember!I41+Jänner!I41+Februar!I41+März!I41</f>
-        <v>161.5</v>
+        <v>174.5</v>
       </c>
     </row>
   </sheetData>
@@ -3937,8 +3937,8 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,10 +4398,12 @@
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4">
+        <v>3</v>
+      </c>
       <c r="I28" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4429,10 +4431,12 @@
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="4">
+        <v>3</v>
+      </c>
       <c r="I30" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4562,7 +4566,7 @@
       </c>
       <c r="I40" s="7">
         <f>I4+I12+I20+I28+I36</f>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4571,7 +4575,7 @@
       </c>
       <c r="I41" s="7">
         <f>I6+I14+I22+I30+I38</f>
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4580,7 +4584,7 @@
       </c>
       <c r="I42" s="7">
         <f>I40+I41</f>
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4593,8 +4597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D867953B-CF18-4E8F-8E2D-D348D0825E5D}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5228,15 +5232,17 @@
         <v>2</v>
       </c>
       <c r="D38" s="4">
-        <v>3</v>
-      </c>
-      <c r="E38" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="E38" s="4">
+        <v>7</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="1"/>
       <c r="I38" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -5257,7 +5263,7 @@
       </c>
       <c r="I41" s="7">
         <f>I6+I14+I22+I30+I38</f>
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5266,7 +5272,7 @@
       </c>
       <c r="I42" s="7">
         <f>I40+I41</f>
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Entwicklung der Seiten aktualisiert
fast fertig, final touches braucht es noch
</commit_message>
<xml_diff>
--- a/Zeiterfassung/Zeiterfassung_Bashar_Metin.xlsx
+++ b/Zeiterfassung/Zeiterfassung_Bashar_Metin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\5.Klasse\SWP\Coding\Diplomarbeit-FahrgemeinschaftenApp\Zeiterfassung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zodia\OneDrive - HTL Dornbirn\5cWI\Z_Diplomarbeit\Diplomarbeit-FahrgemeinschaftenApp\Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C035093C-CD93-4CE3-83AB-D3DCDD52EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFA3549-FC07-4C7B-9DD1-C5D125986F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMME" sheetId="7" r:id="rId1"/>
@@ -575,7 +575,7 @@
       </c>
       <c r="B4">
         <f>September!I41+Oktober!I49+November!I41+Dezember!I41+Jänner!I41+Februar!I41+März!I41</f>
-        <v>181.5</v>
+        <v>187.5</v>
       </c>
     </row>
   </sheetData>
@@ -4614,7 +4614,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5266,12 +5266,16 @@
       <c r="E38" s="4">
         <v>7</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="F38" s="4">
+        <v>2</v>
+      </c>
+      <c r="G38" s="4">
+        <v>4</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="7">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -5292,7 +5296,7 @@
       </c>
       <c r="I41" s="7">
         <f>I6+I14+I22+I30+I38</f>
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5301,7 +5305,7 @@
       </c>
       <c r="I42" s="7">
         <f>I40+I41</f>
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>